<commit_message>
updated docs and BOM
</commit_message>
<xml_diff>
--- a/docs/Kostenberechnung.xlsx
+++ b/docs/Kostenberechnung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Projekte\Elektroauto\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0481BAB-0BC7-4D33-BA9E-2B5D3457C093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F45F27E-3491-4041-AB47-C449B19D8E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{798409B1-55B3-42A6-AF07-6F8A0A9B6A6B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{798409B1-55B3-42A6-AF07-6F8A0A9B6A6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Kosten pro Auto</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Gibt andere ESP32-Boards mit anderen Abmessungen, aber dieses passt bei uns</t>
   </si>
   <si>
-    <t>Noch zu testen, ob der geht</t>
-  </si>
-  <si>
     <t>benutzen glaube ich 6000kV: https://www.banggood.com/de/EMAX-RS1106-II-4500KV-6000KV-7500KV-2~3S-Micro-Brushless-Motor-CCW-Thread-for-RC-Multirotor-FPV-Racing-Drone-p-1177563.html?cur_warehouse=CN&amp;rmmds=search&amp;ID=529815</t>
   </si>
   <si>
@@ -111,12 +108,6 @@
     <t>https://de.aliexpress.com/item/32718555571.html?algo_exp_id=1646453a-ddf1-486b-9dbe-a06ead7f282e-0</t>
   </si>
   <si>
-    <t>https://www.banggood.com/ZOP-Power-7_4V-350mAh-60C-2S-Lipo-Battery-JST-Plug-for-MJX-X401H-X402-JXD-515-515W-515V-RC-Drone-p-1619266.html?cur_warehouse=CN&amp;rmmds=search</t>
-  </si>
-  <si>
-    <t>variieren preislich sehr stark je nach Qualität, Kapazität und Marke (7-15€)</t>
-  </si>
-  <si>
     <t>https://de.aliexpress.com/item/4001184669298.html</t>
   </si>
   <si>
@@ -126,9 +117,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>zur Spannungsglättung für ESC und Arduino, je größer, desto besser (Größenordnung 220-1000µF)</t>
-  </si>
-  <si>
     <t>https://www.conrad.de/de/p/teapo-sy-1000-uf-16-v-10-x-16-mm-elektrolyt-kondensator-radial-bedrahtet-5-mm-1000-f-16-v-20-x-l-10-mm-x-16-mm-443933.html</t>
   </si>
   <si>
@@ -138,7 +126,25 @@
     <t>(war bis vor einiger Zeit noch bei &lt;9€) https://www.banggood.com/de/HAKRC-BLHeli_32-Bit-35A-2-5S-ESC-Built-in-LED-Support-Dshot1200-Multishot-for-FPV-RC-Drone-p-1277587.html?cur_warehouse=CN&amp;rmmds=search</t>
   </si>
   <si>
-    <t>die hier sind leistungsmäßig stark überdimensioniert, aber sehr kompakt</t>
+    <t>alles ab 15A, finde aber leider keine günstigen mehr (Conrad hat gar keine)</t>
+  </si>
+  <si>
+    <t>Suche: "BMI160"</t>
+  </si>
+  <si>
+    <t>zur Spannungsglättung an einen ESC, je größer, desto besser (Größenordnung 220-1000µF)</t>
+  </si>
+  <si>
+    <t>Suche: "Buck converter 3.3V", Input bis mind. 12V muss möglich sein!</t>
+  </si>
+  <si>
+    <t>Preise variieren tagtäglich - ich aktualisier hier die Liste also nicht weiter. Durch den Chipmangel und die neuen Zollrichtlinien sind aber alle Produkte maßlos teurer geworden</t>
+  </si>
+  <si>
+    <t>https://www.conrad.de/de/p/tattu-modellbau-akkupack-lipo-7-4-v-550-mah-zellen-zahl-2-95-c-softcase-2316796.html</t>
+  </si>
+  <si>
+    <t>das non plus ultra und mit 9€ nicht mal teuer</t>
   </si>
 </sst>
 </file>
@@ -519,7 +525,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +534,7 @@
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="92.7109375" customWidth="1"/>
+    <col min="5" max="5" width="83.7109375" customWidth="1"/>
     <col min="6" max="6" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -536,6 +542,9 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -572,19 +581,19 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -602,13 +611,13 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -629,10 +638,10 @@
         <v>15</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -650,10 +659,10 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -671,10 +680,10 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -692,10 +701,10 @@
         <v>1.6</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -703,23 +712,23 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
         <v>0.2</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -737,13 +746,13 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <f>SUM(D4:D11)</f>
-        <v>65</v>
+        <v>64.800000000000011</v>
       </c>
     </row>
   </sheetData>
@@ -757,12 +766,11 @@
     <hyperlink ref="F6" r:id="rId7" xr:uid="{FBD46424-11FC-457C-80A0-FE9E52F1EE9D}"/>
     <hyperlink ref="G6" r:id="rId8" xr:uid="{07B15446-56FC-4FD8-8BF6-CBEF694C8763}"/>
     <hyperlink ref="F7" r:id="rId9" xr:uid="{17246400-0164-4CB1-A675-A2B6F17C3BD2}"/>
-    <hyperlink ref="F8" r:id="rId10" xr:uid="{B0FFE1BA-F7EB-49E6-99CB-C820D1B6B867}"/>
-    <hyperlink ref="F9" r:id="rId11" xr:uid="{26C945EC-D440-454F-846D-969F0BFF195F}"/>
-    <hyperlink ref="F10" r:id="rId12" xr:uid="{F77508C9-C26B-438D-9EFE-19D843B90915}"/>
-    <hyperlink ref="G10" r:id="rId13" xr:uid="{8C7CCC71-54B4-408B-9719-B6188FF7F59B}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{26C945EC-D440-454F-846D-969F0BFF195F}"/>
+    <hyperlink ref="F10" r:id="rId11" xr:uid="{F77508C9-C26B-438D-9EFE-19D843B90915}"/>
+    <hyperlink ref="G10" r:id="rId12" xr:uid="{8C7CCC71-54B4-408B-9719-B6188FF7F59B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>